<commit_message>
didn't commit from home
</commit_message>
<xml_diff>
--- a/HF/data/soot.xlsx
+++ b/HF/data/soot.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoes/GoogleDrive/Shared-w_-Me/Zoe-Sam/soot/HF/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoz\Google Drive\Shared-w_-Me\Zoe-Sam\soot\HF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5140" windowWidth="32700" windowHeight="19740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11580" yWindow="5145" windowWidth="32700" windowHeight="19740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S22" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
   <si>
     <t>CCD</t>
   </si>
@@ -310,15 +310,12 @@
   </si>
   <si>
     <t>Uracil-dimer-stack</t>
-  </si>
-  <si>
-    <t>cp-vdz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000000000"/>
@@ -662,17 +659,17 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="22.375" customWidth="1"/>
+    <col min="7" max="7" width="22.375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -695,7 +692,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -718,7 +715,7 @@
         <v>-44.079704597628101</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -741,7 +738,7 @@
         <v>13.2362952065738</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -764,7 +761,7 @@
         <v>-42.348706934178701</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -787,7 +784,7 @@
         <v>-5.9355185221422504</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
@@ -810,7 +807,7 @@
         <v>0.63225479408618301</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>77</v>
       </c>
@@ -833,7 +830,7 @@
         <v>22.1530345845844</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -856,7 +853,7 @@
         <v>6.1543552599452198</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>79</v>
       </c>
@@ -879,7 +876,7 @@
         <v>-8.4988986670918099</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>80</v>
       </c>
@@ -902,7 +899,7 @@
         <v>4.7691461857294</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>81</v>
       </c>
@@ -925,7 +922,7 @@
         <v>-4.0951007832232298</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -948,7 +945,7 @@
         <v>3.3865762643132999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>83</v>
       </c>
@@ -971,7 +968,7 @@
         <v>-1.8884811921781901</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>84</v>
       </c>
@@ -994,7 +991,7 @@
         <v>-51.235290081841903</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -1017,7 +1014,7 @@
         <v>-64.349335182102607</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -1040,7 +1037,7 @@
         <v>29.116736976261599</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -1063,7 +1060,7 @@
         <v>0.97376670657089903</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -1086,7 +1083,7 @@
         <v>1.49296064430205</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1109,7 +1106,7 @@
         <v>-8.0109017078262603</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1132,7 +1129,7 @@
         <v>17.178197539529801</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1155,7 +1152,7 @@
         <v>-68.356453097236496</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -1178,7 +1175,7 @@
         <v>-0.28629003356883198</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1211,22 +1208,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="3" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.1640625" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.375" customWidth="1"/>
+    <col min="2" max="3" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="19.125" customWidth="1"/>
+    <col min="6" max="6" width="15.625" customWidth="1"/>
+    <col min="7" max="7" width="19.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
@@ -1248,11 +1245,8 @@
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1275,7 +1269,7 @@
         <v>-51.792063588759</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1298,7 +1292,7 @@
         <v>-64.357039449193906</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1321,7 +1315,7 @@
         <v>-65.6670686436468</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1344,7 +1338,7 @@
         <v>-66.101386729919199</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1367,7 +1361,7 @@
         <v>-3.8011841972203499</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1390,7 +1384,7 @@
         <v>5.0013858385699503</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1413,7 +1407,7 @@
         <v>-3.1202037988787699</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1436,7 +1430,7 @@
         <v>16.3414564657113</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1459,7 +1453,7 @@
         <v>5.8733997173353298</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1482,7 +1476,7 @@
         <v>11.7744803435438</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1505,7 +1499,7 @@
         <v>11.8425251644573</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1528,7 +1522,7 @@
         <v>-1.0916776490901201</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>4.3916108379955796</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1574,7 +1568,7 @@
         <v>0.36075000123742001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1597,7 +1591,7 @@
         <v>8.7390964727220499</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1620,7 +1614,7 @@
         <v>1.9385040560209601</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1643,7 +1637,7 @@
         <v>14.912021631591299</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1666,7 +1660,7 @@
         <v>3.7643830887975702</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1689,7 +1683,7 @@
         <v>14.0443700210591</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1706,7 @@
         <v>-3.3621150059414502</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1735,7 +1729,7 @@
         <v>10.710994526014201</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1758,7 +1752,7 @@
         <v>9.5757146733355896</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -1781,7 +1775,7 @@
         <v>7.5020364870729104</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1804,7 +1798,7 @@
         <v>-11.0420291180503</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -1827,7 +1821,7 @@
         <v>-2.2178354643736902</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1850,7 +1844,7 @@
         <v>6.05407927579268</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1873,7 +1867,7 @@
         <v>-9.3283366501776399</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1896,7 +1890,7 @@
         <v>-3.9202293556841799</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1919,7 +1913,7 @@
         <v>-3.9387506828496002</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1942,7 +1936,7 @@
         <v>-6.37771783449098</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1965,7 +1959,7 @@
         <v>1.80446860526542</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1988,7 +1982,7 @@
         <v>-19.066875906732299</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -2011,7 +2005,7 @@
         <v>-17.953405557560501</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -2034,7 +2028,7 @@
         <v>-14.9745098443861</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -2057,7 +2051,7 @@
         <v>-22.085494909819399</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -2080,7 +2074,7 @@
         <v>-17.954219200054499</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -2103,7 +2097,7 @@
         <v>-14.772984340917599</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -2126,7 +2120,7 @@
         <v>6.9438425848275003</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -2149,7 +2143,7 @@
         <v>9.5930870816432599</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -2172,7 +2166,7 @@
         <v>8.8259488003712896</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -2195,7 +2189,7 @@
         <v>8.4904492828990001</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -2218,7 +2212,7 @@
         <v>13.947166397139499</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -2241,7 +2235,7 @@
         <v>2.1496664573325499</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -2264,7 +2258,7 @@
         <v>-14.641344921539099</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2287,7 +2281,7 @@
         <v>-13.364688195022399</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -2310,7 +2304,7 @@
         <v>11.4881669430183</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -2333,7 +2327,7 @@
         <v>-19.5123098351621</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -2356,7 +2350,7 @@
         <v>-14.4412130333807</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -2379,7 +2373,7 @@
         <v>10.860742018796</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -2402,7 +2396,7 @@
         <v>-10.6864970355435</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -2425,7 +2419,7 @@
         <v>-4.9921230744005198</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.95" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -2448,7 +2442,7 @@
         <v>13.7090191070017</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -2471,7 +2465,7 @@
         <v>3.4575301393182598</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -2494,7 +2488,7 @@
         <v>8.3198293275679003</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -2517,7 +2511,7 @@
         <v>12.961676308211199</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -2540,7 +2534,7 @@
         <v>5.6284492313704204</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -2563,7 +2557,7 @@
         <v>1.41611173415836</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -2586,7 +2580,7 @@
         <v>8.4050328412672695</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -2609,7 +2603,7 @@
         <v>14.104236147146</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -2632,7 +2626,7 @@
         <v>-54.080344631146303</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -2655,7 +2649,7 @@
         <v>1.1068827071596801</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>67</v>
       </c>
@@ -2678,7 +2672,7 @@
         <v>-19.437819411709601</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>68</v>
       </c>
@@ -2701,7 +2695,7 @@
         <v>-15.71310972833</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>69</v>
       </c>
@@ -2724,7 +2718,7 @@
         <v>-24.3803919497891</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2747,7 +2741,7 @@
         <v>-18.723277509453499</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>71</v>
       </c>

</xml_diff>